<commit_message>
Updating to Version 1.3
</commit_message>
<xml_diff>
--- a/FFRMS_RasterQC_Configuration.xlsx
+++ b/FFRMS_RasterQC_Configuration.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="26529"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="26626"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\FFRMS\Raster_QC_Tool\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\FFRMS\Raster_QC_Tool\FFRMS_Raster_QC_Tool\FFRMS_RasterQC_Tool_V1.2\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6F7765C7-1DBD-4E0B-AE63-F35E09E29726}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DE19C9CA-F758-4172-A433-FA142EE4FF9B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="8835" yWindow="1635" windowWidth="19020" windowHeight="11385" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="RasterCompare" sheetId="1" r:id="rId1"/>
@@ -51,15 +51,6 @@
     <t>OutputSpreadSheet</t>
   </si>
   <si>
-    <t>FFRNS 0.2% ACF raster</t>
-  </si>
-  <si>
-    <t>GRAYS_HARBOR_Riverine_Raster_QC_Result</t>
-  </si>
-  <si>
-    <t>Please include full folder path, raster name and extention(.tif)</t>
-  </si>
-  <si>
     <t>Name only. CSV will generate under script folder</t>
   </si>
   <si>
@@ -75,7 +66,16 @@
     <t>D:\...\Raster\WA_53027C_10N_03FVA_RIV_03m.tif</t>
   </si>
   <si>
-    <t>D:\...\Raster\WA_53027C_10N_0_2PCT_RIV_03m.tif</t>
+    <t>XXX_Riverine_Raster_QC_Result</t>
+  </si>
+  <si>
+    <t>Leave it blank if there is no 0.2% raster in this project</t>
+  </si>
+  <si>
+    <t>Please include full folder path, raster name and extention(.tif) for rasters</t>
+  </si>
+  <si>
+    <t>FFRMS 0.2% ACF raster</t>
   </si>
 </sst>
 </file>
@@ -433,7 +433,7 @@
   <dimension ref="A1:C7"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B11" sqref="B11"/>
+      <selection activeCell="B8" sqref="B8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -454,15 +454,15 @@
         <v>2</v>
       </c>
     </row>
-    <row r="2" spans="1:3" ht="30" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A2" s="2" t="s">
         <v>3</v>
       </c>
       <c r="B2" s="4" t="s">
-        <v>12</v>
+        <v>9</v>
       </c>
       <c r="C2" s="3" t="s">
-        <v>10</v>
+        <v>15</v>
       </c>
     </row>
     <row r="3" spans="1:3" x14ac:dyDescent="0.25">
@@ -470,7 +470,7 @@
         <v>4</v>
       </c>
       <c r="B3" s="4" t="s">
-        <v>13</v>
+        <v>10</v>
       </c>
       <c r="C3" s="3"/>
     </row>
@@ -479,7 +479,7 @@
         <v>5</v>
       </c>
       <c r="B4" s="4" t="s">
-        <v>14</v>
+        <v>11</v>
       </c>
       <c r="C4" s="3"/>
     </row>
@@ -488,28 +488,28 @@
         <v>6</v>
       </c>
       <c r="B5" s="4" t="s">
-        <v>15</v>
+        <v>12</v>
       </c>
       <c r="C5" s="1"/>
     </row>
     <row r="6" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A6" s="2" t="s">
-        <v>8</v>
-      </c>
-      <c r="B6" s="4" t="s">
         <v>16</v>
       </c>
-      <c r="C6" s="3"/>
+      <c r="B6" s="4"/>
+      <c r="C6" s="3" t="s">
+        <v>14</v>
+      </c>
     </row>
     <row r="7" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A7" s="2" t="s">
         <v>7</v>
       </c>
       <c r="B7" s="4" t="s">
-        <v>9</v>
+        <v>13</v>
       </c>
       <c r="C7" s="3" t="s">
-        <v>11</v>
+        <v>8</v>
       </c>
     </row>
   </sheetData>

</xml_diff>